<commit_message>
Added tests for search and lookup
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SearchTermData.xlsx
+++ b/src/test/resources/testdata/SearchTermData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikander.raja/Documents/SCM_AUTOMATION/scm-platform/AjioB2C/fs/ITunesSearchTest/src/test/resources/com.apple.developer.itunes.search.api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikander.raja/Documents/SCM_AUTOMATION/scm-platform/AjioB2C/srdemo/ITunesSearchTest/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16DBF5A-6CB2-8F4A-991E-69F624BDC85D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D86C6BC-1AF5-144C-BC69-DD310E9CA559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{0158ACA4-F70A-A842-83A6-8CFE25178742}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{0158ACA4-F70A-A842-83A6-8CFE25178742}"/>
   </bookViews>
   <sheets>
     <sheet name="SEARCH_TERM" sheetId="1" r:id="rId1"/>
+    <sheet name="LOOKUP_TERM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>term</t>
   </si>
@@ -48,9 +49,6 @@
     <t>ca</t>
   </si>
   <si>
-    <t>jim+jones</t>
-  </si>
-  <si>
     <t>yelp</t>
   </si>
   <si>
@@ -58,6 +56,93 @@
   </si>
   <si>
     <t>software</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>podcast</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>audiobook</t>
+  </si>
+  <si>
+    <t>shortFilm</t>
+  </si>
+  <si>
+    <t>tvShow</t>
+  </si>
+  <si>
+    <t>ebook</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>ja_jp</t>
+  </si>
+  <si>
+    <t>en_us</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>amgArtistId</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>upc</t>
+  </si>
+  <si>
+    <t>amgVideoId</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>468749,5723</t>
+  </si>
+  <si>
+    <t>468749</t>
+  </si>
+  <si>
+    <t>909253</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>68749,5723</t>
+  </si>
+  <si>
+    <t>song</t>
+  </si>
+  <si>
+    <t>recent</t>
+  </si>
+  <si>
+    <t>720642462928</t>
+  </si>
+  <si>
+    <t>15175,15176,15177,15178,15183,15184,15187,1519,15191,15195,15197,15198</t>
+  </si>
+  <si>
+    <t>amgAlbumId</t>
+  </si>
+  <si>
+    <t>17120</t>
   </si>
 </sst>
 </file>
@@ -116,10 +201,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,18 +522,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7F10EA-7B70-A74E-B88E-4A5FB4A52616}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -458,8 +547,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -468,46 +563,354 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC40D969-EEFF-0941-B5B9-B7FEB5181539}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>909253</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>284910350</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Separated test data and fixed validation issue
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SearchTermData.xlsx
+++ b/src/test/resources/testdata/SearchTermData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikander.raja/Documents/SCM_AUTOMATION/scm-platform/AjioB2C/srdemo/ITunesSearchTest/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D86C6BC-1AF5-144C-BC69-DD310E9CA559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8E2AA9-745F-6E45-B05D-7910CFB2DBD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{0158ACA4-F70A-A842-83A6-8CFE25178742}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>term</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>17120</t>
+  </si>
+  <si>
+    <t>9780316069359</t>
   </si>
 </sst>
 </file>
@@ -733,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC40D969-EEFF-0941-B5B9-B7FEB5181539}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,6 +912,19 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>